<commit_message>
affiliation and study area map
</commit_message>
<xml_diff>
--- a/datasets/Cleaned_data.xlsx
+++ b/datasets/Cleaned_data.xlsx
@@ -2569,7 +2569,7 @@
     <t xml:space="preserve">P026</t>
   </si>
   <si>
-    <t xml:space="preserve">Fuenlabra, Spain</t>
+    <t xml:space="preserve">Fuenlabrada, Spain</t>
   </si>
   <si>
     <t xml:space="preserve">Sensor data</t>
@@ -8190,8 +8190,8 @@
   </sheetPr>
   <dimension ref="A1:AZ142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AJ40" activeCellId="0" sqref="AJ40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Y25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AJ38" activeCellId="0" sqref="AJ38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11019,11 +11019,11 @@
       <c r="AK19" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL19" s="3" t="b">
+      <c r="AL19" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM19" s="3" t="b">
+      <c r="AM19" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11042,11 +11042,11 @@
       <c r="AR19" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AS19" s="3" t="b">
+      <c r="AS19" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU19" s="3" t="b">
+      <c r="AU19" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -11169,11 +11169,11 @@
       <c r="AK20" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL20" s="3" t="b">
+      <c r="AL20" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM20" s="3" t="b">
+      <c r="AM20" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11189,11 +11189,11 @@
       <c r="AR20" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="AS20" s="3" t="b">
+      <c r="AS20" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU20" s="3" t="b">
+      <c r="AU20" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11316,11 +11316,11 @@
       <c r="AK21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL21" s="3" t="b">
+      <c r="AL21" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM21" s="3" t="b">
+      <c r="AM21" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11339,11 +11339,11 @@
       <c r="AR21" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="AS21" s="3" t="b">
+      <c r="AS21" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU21" s="3" t="b">
+      <c r="AU21" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11469,11 +11469,11 @@
       <c r="AK22" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL22" s="3" t="b">
+      <c r="AL22" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM22" s="3" t="b">
+      <c r="AM22" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11489,11 +11489,11 @@
       <c r="AR22" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AS22" s="3" t="b">
+      <c r="AS22" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU22" s="3" t="b">
+      <c r="AU22" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -11616,11 +11616,11 @@
       <c r="AK23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL23" s="3" t="b">
+      <c r="AL23" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM23" s="3" t="b">
+      <c r="AM23" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11636,14 +11636,14 @@
       <c r="AR23" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="AS23" s="3" t="b">
+      <c r="AS23" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT23" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="AU23" s="3" t="b">
+      <c r="AU23" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11766,11 +11766,11 @@
       <c r="AK24" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL24" s="3" t="b">
+      <c r="AL24" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM24" s="3" t="b">
+      <c r="AM24" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11786,11 +11786,11 @@
       <c r="AR24" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="AS24" s="3" t="b">
+      <c r="AS24" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU24" s="3" t="b">
+      <c r="AU24" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11919,11 +11919,11 @@
       <c r="AK25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL25" s="3" t="b">
+      <c r="AL25" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM25" s="3" t="b">
+      <c r="AM25" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11942,11 +11942,11 @@
       <c r="AR25" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AS25" s="3" t="b">
+      <c r="AS25" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU25" s="3" t="b">
+      <c r="AU25" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12072,11 +12072,11 @@
       <c r="AK26" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL26" s="3" t="b">
+      <c r="AL26" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM26" s="3" t="b">
+      <c r="AM26" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12092,14 +12092,14 @@
       <c r="AR26" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="AS26" s="3" t="b">
+      <c r="AS26" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT26" s="2" t="s">
         <v>638</v>
       </c>
-      <c r="AU26" s="3" t="b">
+      <c r="AU26" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -12222,11 +12222,11 @@
       <c r="AK27" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL27" s="3" t="b">
+      <c r="AL27" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM27" s="3" t="b">
+      <c r="AM27" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -12245,14 +12245,14 @@
       <c r="AR27" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="AS27" s="3" t="b">
+      <c r="AS27" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="AT27" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="AU27" s="3" t="b">
+      <c r="AU27" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12378,11 +12378,11 @@
       <c r="AK28" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL28" s="3" t="b">
+      <c r="AL28" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM28" s="3" t="b">
+      <c r="AM28" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12401,11 +12401,11 @@
       <c r="AR28" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="AS28" s="3" t="b">
+      <c r="AS28" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU28" s="3" t="b">
+      <c r="AU28" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12519,11 +12519,11 @@
       <c r="AJ29" s="2" t="s">
         <v>706</v>
       </c>
-      <c r="AL29" s="3" t="b">
+      <c r="AL29" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM29" s="3" t="b">
+      <c r="AM29" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12542,11 +12542,11 @@
       <c r="AR29" s="2" t="s">
         <v>710</v>
       </c>
-      <c r="AS29" s="3" t="b">
+      <c r="AS29" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU29" s="3" t="b">
+      <c r="AU29" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12672,11 +12672,11 @@
       <c r="AK30" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL30" s="3" t="b">
+      <c r="AL30" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM30" s="3" t="b">
+      <c r="AM30" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12692,11 +12692,11 @@
       <c r="AR30" s="2" t="s">
         <v>729</v>
       </c>
-      <c r="AS30" s="3" t="b">
+      <c r="AS30" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU30" s="3" t="b">
+      <c r="AU30" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12822,11 +12822,11 @@
       <c r="AK31" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL31" s="3" t="b">
+      <c r="AL31" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM31" s="3" t="b">
+      <c r="AM31" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12845,11 +12845,11 @@
       <c r="AR31" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AS31" s="3" t="b">
+      <c r="AS31" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU31" s="3" t="b">
+      <c r="AU31" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -12960,11 +12960,11 @@
       <c r="AK32" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL32" s="3" t="b">
+      <c r="AL32" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM32" s="3" t="b">
+      <c r="AM32" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12983,11 +12983,11 @@
       <c r="AR32" s="2" t="s">
         <v>764</v>
       </c>
-      <c r="AS32" s="3" t="b">
+      <c r="AS32" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU32" s="3" t="b">
+      <c r="AU32" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -13119,11 +13119,11 @@
       <c r="AK33" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL33" s="3" t="b">
+      <c r="AL33" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM33" s="3" t="b">
+      <c r="AM33" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13139,11 +13139,11 @@
       <c r="AR33" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="AS33" s="3" t="b">
+      <c r="AS33" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU33" s="3" t="b">
+      <c r="AU33" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13266,11 +13266,11 @@
       <c r="AK34" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL34" s="3" t="b">
+      <c r="AL34" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM34" s="3" t="b">
+      <c r="AM34" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13289,11 +13289,11 @@
       <c r="AR34" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="AS34" s="3" t="b">
+      <c r="AS34" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU34" s="3" t="b">
+      <c r="AU34" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13419,11 +13419,11 @@
       <c r="AK35" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="AL35" s="3" t="b">
+      <c r="AL35" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM35" s="3" t="b">
+      <c r="AM35" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -13439,11 +13439,11 @@
       <c r="AR35" s="2" t="s">
         <v>820</v>
       </c>
-      <c r="AS35" s="3" t="b">
+      <c r="AS35" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU35" s="3" t="b">
+      <c r="AU35" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -13560,11 +13560,11 @@
       <c r="AK36" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL36" s="3" t="b">
+      <c r="AL36" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM36" s="3" t="b">
+      <c r="AM36" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13583,11 +13583,11 @@
       <c r="AR36" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AS36" s="3" t="b">
+      <c r="AS36" s="2" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU36" s="3" t="b">
+      <c r="AU36" s="2" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -16851,11 +16851,11 @@
       <c r="AK58" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL58" s="1" t="b">
+      <c r="AL58" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM58" s="1" t="b">
+      <c r="AM58" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -16871,11 +16871,11 @@
       <c r="AR58" s="2" t="s">
         <v>1233</v>
       </c>
-      <c r="AS58" s="1" t="b">
+      <c r="AS58" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU58" s="1" t="b">
+      <c r="AU58" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -16995,11 +16995,11 @@
       <c r="AK59" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL59" s="1" t="b">
+      <c r="AL59" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM59" s="1" t="b">
+      <c r="AM59" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -17015,11 +17015,11 @@
       <c r="AR59" s="2" t="s">
         <v>1256</v>
       </c>
-      <c r="AS59" s="1" t="b">
+      <c r="AS59" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU59" s="1" t="b">
+      <c r="AU59" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17142,11 +17142,11 @@
       <c r="AK60" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL60" s="1" t="b">
+      <c r="AL60" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM60" s="1" t="b">
+      <c r="AM60" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -17162,11 +17162,11 @@
       <c r="AR60" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AS60" s="1" t="b">
+      <c r="AS60" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU60" s="1" t="b">
+      <c r="AU60" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17289,11 +17289,11 @@
       <c r="AK61" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL61" s="1" t="b">
+      <c r="AL61" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM61" s="1" t="b">
+      <c r="AM61" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17312,11 +17312,11 @@
       <c r="AR61" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="AS61" s="1" t="b">
+      <c r="AS61" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU61" s="1" t="b">
+      <c r="AU61" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17439,11 +17439,11 @@
       <c r="AK62" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL62" s="1" t="b">
+      <c r="AL62" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM62" s="1" t="b">
+      <c r="AM62" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -17459,14 +17459,14 @@
       <c r="AR62" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AS62" s="1" t="b">
+      <c r="AS62" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="AT62" s="2" t="s">
         <v>1316</v>
       </c>
-      <c r="AU62" s="1" t="b">
+      <c r="AU62" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -17589,11 +17589,11 @@
       <c r="AK63" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL63" s="1" t="b">
+      <c r="AL63" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM63" s="1" t="b">
+      <c r="AM63" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -17609,11 +17609,11 @@
       <c r="AR63" s="2" t="s">
         <v>1334</v>
       </c>
-      <c r="AS63" s="1" t="b">
+      <c r="AS63" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU63" s="1" t="b">
+      <c r="AU63" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -17727,11 +17727,11 @@
       <c r="AK64" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL64" s="1" t="b">
+      <c r="AL64" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM64" s="1" t="b">
+      <c r="AM64" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -17750,11 +17750,11 @@
       <c r="AR64" s="2" t="s">
         <v>1135</v>
       </c>
-      <c r="AS64" s="1" t="b">
+      <c r="AS64" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU64" s="1" t="b">
+      <c r="AU64" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -17877,11 +17877,11 @@
       <c r="AK65" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL65" s="1" t="b">
+      <c r="AL65" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM65" s="1" t="b">
+      <c r="AM65" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -17897,11 +17897,11 @@
       <c r="AR65" s="2" t="s">
         <v>1365</v>
       </c>
-      <c r="AS65" s="1" t="b">
+      <c r="AS65" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU65" s="1" t="b">
+      <c r="AU65" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18021,11 +18021,11 @@
       <c r="AK66" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL66" s="1" t="b">
+      <c r="AL66" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM66" s="1" t="b">
+      <c r="AM66" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -18041,11 +18041,11 @@
       <c r="AR66" s="2" t="s">
         <v>1380</v>
       </c>
-      <c r="AS66" s="1" t="b">
+      <c r="AS66" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU66" s="1" t="b">
+      <c r="AU66" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -18162,11 +18162,11 @@
       <c r="AK67" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL67" s="1" t="b">
+      <c r="AL67" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM67" s="1" t="b">
+      <c r="AM67" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -18182,11 +18182,11 @@
       <c r="AR67" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="AS67" s="1" t="b">
+      <c r="AS67" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU67" s="1" t="b">
+      <c r="AU67" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -18309,11 +18309,11 @@
       <c r="AK68" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL68" s="1" t="b">
+      <c r="AL68" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM68" s="1" t="b">
+      <c r="AM68" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18332,14 +18332,14 @@
       <c r="AR68" s="2" t="s">
         <v>1417</v>
       </c>
-      <c r="AS68" s="1" t="b">
+      <c r="AS68" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT68" s="2" t="s">
         <v>1418</v>
       </c>
-      <c r="AU68" s="1" t="b">
+      <c r="AU68" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18453,11 +18453,11 @@
       <c r="AK69" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL69" s="1" t="b">
+      <c r="AL69" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM69" s="1" t="b">
+      <c r="AM69" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -18476,11 +18476,11 @@
       <c r="AR69" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AS69" s="1" t="b">
+      <c r="AS69" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU69" s="1" t="b">
+      <c r="AU69" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -18609,11 +18609,11 @@
       <c r="AK70" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="AL70" s="1" t="b">
+      <c r="AL70" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM70" s="1" t="b">
+      <c r="AM70" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -18632,11 +18632,11 @@
       <c r="AR70" s="2" t="s">
         <v>1456</v>
       </c>
-      <c r="AS70" s="1" t="b">
+      <c r="AS70" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU70" s="1" t="b">
+      <c r="AU70" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -18759,11 +18759,11 @@
       <c r="AK71" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL71" s="1" t="b">
+      <c r="AL71" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM71" s="1" t="b">
+      <c r="AM71" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -18782,11 +18782,11 @@
       <c r="AR71" s="2" t="s">
         <v>1473</v>
       </c>
-      <c r="AS71" s="1" t="b">
+      <c r="AS71" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU71" s="1" t="b">
+      <c r="AU71" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -18909,11 +18909,11 @@
       <c r="AK72" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL72" s="1" t="b">
+      <c r="AL72" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM72" s="1" t="b">
+      <c r="AM72" s="4" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -18929,11 +18929,11 @@
       <c r="AR72" s="2" t="s">
         <v>764</v>
       </c>
-      <c r="AS72" s="1" t="b">
+      <c r="AS72" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU72" s="1" t="b">
+      <c r="AU72" s="4" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -19503,11 +19503,11 @@
       <c r="AK76" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL76" s="4" t="b">
+      <c r="AL76" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM76" s="4" t="b">
+      <c r="AM76" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -19526,14 +19526,14 @@
       <c r="AR76" s="2" t="s">
         <v>1569</v>
       </c>
-      <c r="AS76" s="4" t="b">
+      <c r="AS76" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT76" s="2" t="s">
         <v>1570</v>
       </c>
-      <c r="AU76" s="4" t="b">
+      <c r="AU76" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -19659,11 +19659,11 @@
       <c r="AK77" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL77" s="4" t="b">
+      <c r="AL77" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM77" s="4" t="b">
+      <c r="AM77" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -19682,11 +19682,11 @@
       <c r="AR77" s="2" t="s">
         <v>1592</v>
       </c>
-      <c r="AS77" s="4" t="b">
+      <c r="AS77" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU77" s="4" t="b">
+      <c r="AU77" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -19809,11 +19809,11 @@
       <c r="AK78" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL78" s="4" t="b">
+      <c r="AL78" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM78" s="4" t="b">
+      <c r="AM78" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -19832,11 +19832,11 @@
       <c r="AR78" s="2" t="s">
         <v>1610</v>
       </c>
-      <c r="AS78" s="4" t="b">
+      <c r="AS78" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU78" s="4" t="b">
+      <c r="AU78" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -19962,11 +19962,11 @@
       <c r="AK79" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL79" s="4" t="b">
+      <c r="AL79" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM79" s="4" t="b">
+      <c r="AM79" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -19985,11 +19985,11 @@
       <c r="AR79" s="2" t="s">
         <v>1632</v>
       </c>
-      <c r="AS79" s="4" t="b">
+      <c r="AS79" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU79" s="4" t="b">
+      <c r="AU79" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20106,11 +20106,11 @@
       <c r="AK80" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL80" s="4" t="b">
+      <c r="AL80" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM80" s="4" t="b">
+      <c r="AM80" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20129,11 +20129,11 @@
       <c r="AR80" s="2" t="s">
         <v>907</v>
       </c>
-      <c r="AS80" s="4" t="b">
+      <c r="AS80" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU80" s="4" t="b">
+      <c r="AU80" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -20253,11 +20253,11 @@
       <c r="AK81" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL81" s="4" t="b">
+      <c r="AL81" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM81" s="4" t="b">
+      <c r="AM81" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -20276,14 +20276,14 @@
       <c r="AR81" s="2" t="s">
         <v>1662</v>
       </c>
-      <c r="AS81" s="4" t="b">
+      <c r="AS81" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT81" s="2" t="s">
         <v>1663</v>
       </c>
-      <c r="AU81" s="4" t="b">
+      <c r="AU81" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -20409,11 +20409,11 @@
       <c r="AK82" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL82" s="4" t="b">
+      <c r="AL82" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM82" s="4" t="b">
+      <c r="AM82" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -20432,11 +20432,11 @@
       <c r="AR82" s="2" t="s">
         <v>1687</v>
       </c>
-      <c r="AS82" s="4" t="b">
+      <c r="AS82" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU82" s="4" t="b">
+      <c r="AU82" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20559,11 +20559,11 @@
       <c r="AK83" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL83" s="4" t="b">
+      <c r="AL83" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM83" s="4" t="b">
+      <c r="AM83" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -20579,11 +20579,11 @@
       <c r="AR83" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AS83" s="4" t="b">
+      <c r="AS83" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU83" s="4" t="b">
+      <c r="AU83" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20709,11 +20709,11 @@
       <c r="AK84" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL84" s="4" t="b">
+      <c r="AL84" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM84" s="4" t="b">
+      <c r="AM84" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -20732,11 +20732,11 @@
       <c r="AR84" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="AS84" s="4" t="b">
+      <c r="AS84" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU84" s="4" t="b">
+      <c r="AU84" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -20862,11 +20862,11 @@
       <c r="AK85" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL85" s="4" t="b">
+      <c r="AL85" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM85" s="4" t="b">
+      <c r="AM85" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -20882,11 +20882,11 @@
       <c r="AR85" s="2" t="s">
         <v>1171</v>
       </c>
-      <c r="AS85" s="4" t="b">
+      <c r="AS85" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU85" s="4" t="b">
+      <c r="AU85" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -21012,11 +21012,11 @@
       <c r="AK86" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="AL86" s="4" t="b">
+      <c r="AL86" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM86" s="4" t="b">
+      <c r="AM86" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21035,11 +21035,11 @@
       <c r="AR86" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="AS86" s="4" t="b">
+      <c r="AS86" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU86" s="4" t="b">
+      <c r="AU86" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -21159,11 +21159,11 @@
       <c r="AK87" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL87" s="4" t="b">
+      <c r="AL87" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM87" s="4" t="b">
+      <c r="AM87" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -21179,11 +21179,11 @@
       <c r="AR87" s="2" t="s">
         <v>907</v>
       </c>
-      <c r="AS87" s="4" t="b">
+      <c r="AS87" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU87" s="4" t="b">
+      <c r="AU87" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -21294,11 +21294,11 @@
       <c r="AK88" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL88" s="4" t="b">
+      <c r="AL88" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM88" s="4" t="b">
+      <c r="AM88" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -21314,11 +21314,11 @@
       <c r="AR88" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="AS88" s="4" t="b">
+      <c r="AS88" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU88" s="4" t="b">
+      <c r="AU88" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21435,11 +21435,11 @@
       <c r="AK89" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL89" s="4" t="b">
+      <c r="AL89" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM89" s="4" t="b">
+      <c r="AM89" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -21458,11 +21458,11 @@
       <c r="AR89" s="2" t="s">
         <v>1806</v>
       </c>
-      <c r="AS89" s="4" t="b">
+      <c r="AS89" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU89" s="4" t="b">
+      <c r="AU89" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -21585,11 +21585,11 @@
       <c r="AK90" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL90" s="4" t="b">
+      <c r="AL90" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM90" s="4" t="b">
+      <c r="AM90" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -21605,14 +21605,14 @@
       <c r="AR90" s="2" t="s">
         <v>1821</v>
       </c>
-      <c r="AS90" s="4" t="b">
+      <c r="AS90" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT90" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="AU90" s="4" t="b">
+      <c r="AU90" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -21735,11 +21735,11 @@
       <c r="AK91" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL91" s="4" t="b">
+      <c r="AL91" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM91" s="4" t="b">
+      <c r="AM91" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -21758,14 +21758,14 @@
       <c r="AR91" s="2" t="s">
         <v>1838</v>
       </c>
-      <c r="AS91" s="4" t="b">
+      <c r="AS91" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT91" s="2" t="s">
         <v>1839</v>
       </c>
-      <c r="AU91" s="4" t="b">
+      <c r="AU91" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -21891,11 +21891,11 @@
       <c r="AK92" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL92" s="4" t="b">
+      <c r="AL92" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM92" s="4" t="b">
+      <c r="AM92" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -21911,11 +21911,11 @@
       <c r="AR92" s="2" t="s">
         <v>1857</v>
       </c>
-      <c r="AS92" s="4" t="b">
+      <c r="AS92" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU92" s="4" t="b">
+      <c r="AU92" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -22041,11 +22041,11 @@
       <c r="AK93" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL93" s="4" t="b">
+      <c r="AL93" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM93" s="4" t="b">
+      <c r="AM93" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22064,11 +22064,11 @@
       <c r="AR93" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AS93" s="4" t="b">
+      <c r="AS93" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU93" s="4" t="b">
+      <c r="AU93" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -22197,11 +22197,11 @@
       <c r="AK94" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL94" s="4" t="b">
+      <c r="AL94" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM94" s="4" t="b">
+      <c r="AM94" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22220,11 +22220,11 @@
       <c r="AR94" s="2" t="s">
         <v>1902</v>
       </c>
-      <c r="AS94" s="4" t="b">
+      <c r="AS94" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU94" s="4" t="b">
+      <c r="AU94" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22353,11 +22353,11 @@
       <c r="AK95" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL95" s="4" t="b">
+      <c r="AL95" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM95" s="4" t="b">
+      <c r="AM95" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -22373,11 +22373,11 @@
       <c r="AR95" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AS95" s="4" t="b">
+      <c r="AS95" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU95" s="4" t="b">
+      <c r="AU95" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22494,11 +22494,11 @@
       <c r="AK96" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL96" s="4" t="b">
+      <c r="AL96" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM96" s="4" t="b">
+      <c r="AM96" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -22514,11 +22514,11 @@
       <c r="AR96" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AS96" s="4" t="b">
+      <c r="AS96" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU96" s="4" t="b">
+      <c r="AU96" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -22635,11 +22635,11 @@
       <c r="AK97" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL97" s="4" t="b">
+      <c r="AL97" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM97" s="4" t="b">
+      <c r="AM97" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -22658,11 +22658,11 @@
       <c r="AR97" s="2" t="s">
         <v>1949</v>
       </c>
-      <c r="AS97" s="4" t="b">
+      <c r="AS97" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU97" s="4" t="b">
+      <c r="AU97" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -22785,11 +22785,11 @@
       <c r="AK98" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL98" s="4" t="b">
+      <c r="AL98" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM98" s="4" t="b">
+      <c r="AM98" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22808,11 +22808,11 @@
       <c r="AR98" s="2" t="s">
         <v>1096</v>
       </c>
-      <c r="AS98" s="4" t="b">
+      <c r="AS98" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU98" s="4" t="b">
+      <c r="AU98" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -22935,11 +22935,11 @@
       <c r="AK99" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL99" s="4" t="b">
+      <c r="AL99" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM99" s="4" t="b">
+      <c r="AM99" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -22955,11 +22955,11 @@
       <c r="AR99" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AS99" s="4" t="b">
+      <c r="AS99" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU99" s="4" t="b">
+      <c r="AU99" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23079,11 +23079,11 @@
       <c r="AK100" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="AL100" s="4" t="b">
+      <c r="AL100" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM100" s="4" t="b">
+      <c r="AM100" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23099,11 +23099,11 @@
       <c r="AR100" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AS100" s="4" t="b">
+      <c r="AS100" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU100" s="4" t="b">
+      <c r="AU100" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23220,11 +23220,11 @@
       <c r="AK101" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL101" s="4" t="b">
+      <c r="AL101" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM101" s="4" t="b">
+      <c r="AM101" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23240,14 +23240,14 @@
       <c r="AR101" s="2" t="s">
         <v>2019</v>
       </c>
-      <c r="AS101" s="4" t="b">
+      <c r="AS101" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT101" s="2" t="s">
         <v>2020</v>
       </c>
-      <c r="AU101" s="4" t="b">
+      <c r="AU101" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23364,11 +23364,11 @@
       <c r="AK102" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL102" s="4" t="b">
+      <c r="AL102" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM102" s="4" t="b">
+      <c r="AM102" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23384,11 +23384,11 @@
       <c r="AR102" s="2" t="s">
         <v>2042</v>
       </c>
-      <c r="AS102" s="4" t="b">
+      <c r="AS102" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU102" s="4" t="b">
+      <c r="AU102" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23517,11 +23517,11 @@
       <c r="AK103" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL103" s="4" t="b">
+      <c r="AL103" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM103" s="4" t="b">
+      <c r="AM103" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23537,11 +23537,11 @@
       <c r="AR103" s="2" t="s">
         <v>907</v>
       </c>
-      <c r="AS103" s="4" t="b">
+      <c r="AS103" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU103" s="4" t="b">
+      <c r="AU103" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23661,11 +23661,11 @@
       <c r="AK104" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL104" s="4" t="b">
+      <c r="AL104" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM104" s="4" t="b">
+      <c r="AM104" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23681,11 +23681,11 @@
       <c r="AR104" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AS104" s="4" t="b">
+      <c r="AS104" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU104" s="4" t="b">
+      <c r="AU104" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23799,11 +23799,11 @@
       <c r="AK105" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL105" s="4" t="b">
+      <c r="AL105" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM105" s="4" t="b">
+      <c r="AM105" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23822,11 +23822,11 @@
       <c r="AR105" s="2" t="s">
         <v>1838</v>
       </c>
-      <c r="AS105" s="4" t="b">
+      <c r="AS105" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU105" s="4" t="b">
+      <c r="AU105" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23949,11 +23949,11 @@
       <c r="AK106" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL106" s="4" t="b">
+      <c r="AL106" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM106" s="4" t="b">
+      <c r="AM106" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -23972,11 +23972,11 @@
       <c r="AR106" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AS106" s="4" t="b">
+      <c r="AS106" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU106" s="4" t="b">
+      <c r="AU106" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24099,11 +24099,11 @@
       <c r="AK107" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="AL107" s="4" t="b">
+      <c r="AL107" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM107" s="4" t="b">
+      <c r="AM107" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -24119,11 +24119,11 @@
       <c r="AR107" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AS107" s="4" t="b">
+      <c r="AS107" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU107" s="4" t="b">
+      <c r="AU107" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24246,11 +24246,11 @@
       <c r="AK108" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL108" s="4" t="b">
+      <c r="AL108" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM108" s="4" t="b">
+      <c r="AM108" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -24269,11 +24269,11 @@
       <c r="AR108" s="2" t="s">
         <v>1048</v>
       </c>
-      <c r="AS108" s="4" t="b">
+      <c r="AS108" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU108" s="4" t="b">
+      <c r="AU108" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24396,11 +24396,11 @@
       <c r="AK109" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL109" s="4" t="b">
+      <c r="AL109" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM109" s="4" t="b">
+      <c r="AM109" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -24419,11 +24419,11 @@
       <c r="AR109" s="2" t="s">
         <v>2165</v>
       </c>
-      <c r="AS109" s="4" t="b">
+      <c r="AS109" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU109" s="4" t="b">
+      <c r="AU109" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24546,11 +24546,11 @@
       <c r="AK110" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL110" s="4" t="b">
+      <c r="AL110" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM110" s="4" t="b">
+      <c r="AM110" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -24569,14 +24569,14 @@
       <c r="AR110" s="2" t="s">
         <v>1256</v>
       </c>
-      <c r="AS110" s="4" t="b">
+      <c r="AS110" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT110" s="2" t="s">
         <v>2181</v>
       </c>
-      <c r="AU110" s="4" t="b">
+      <c r="AU110" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24699,11 +24699,11 @@
       <c r="AK111" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="AL111" s="4" t="b">
+      <c r="AL111" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM111" s="4" t="b">
+      <c r="AM111" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -24719,11 +24719,11 @@
       <c r="AR111" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AS111" s="4" t="b">
+      <c r="AS111" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU111" s="4" t="b">
+      <c r="AU111" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24843,11 +24843,11 @@
       <c r="AK112" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL112" s="4" t="b">
+      <c r="AL112" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM112" s="4" t="b">
+      <c r="AM112" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -24866,11 +24866,11 @@
       <c r="AR112" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="AS112" s="4" t="b">
+      <c r="AS112" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU112" s="4" t="b">
+      <c r="AU112" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -24993,11 +24993,11 @@
       <c r="AK113" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL113" s="4" t="b">
+      <c r="AL113" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM113" s="4" t="b">
+      <c r="AM113" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25016,11 +25016,11 @@
       <c r="AR113" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AS113" s="4" t="b">
+      <c r="AS113" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU113" s="4" t="b">
+      <c r="AU113" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25137,11 +25137,11 @@
       <c r="AK114" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL114" s="4" t="b">
+      <c r="AL114" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM114" s="4" t="b">
+      <c r="AM114" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25157,11 +25157,11 @@
       <c r="AR114" s="2" t="s">
         <v>2243</v>
       </c>
-      <c r="AS114" s="4" t="b">
+      <c r="AS114" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU114" s="4" t="b">
+      <c r="AU114" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25275,11 +25275,11 @@
       <c r="AK115" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL115" s="4" t="b">
+      <c r="AL115" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM115" s="4" t="b">
+      <c r="AM115" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25295,11 +25295,11 @@
       <c r="AR115" s="2" t="s">
         <v>2263</v>
       </c>
-      <c r="AS115" s="4" t="b">
+      <c r="AS115" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU115" s="4" t="b">
+      <c r="AU115" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25422,11 +25422,11 @@
       <c r="AK116" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL116" s="4" t="b">
+      <c r="AL116" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM116" s="4" t="b">
+      <c r="AM116" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25445,11 +25445,11 @@
       <c r="AR116" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AS116" s="4" t="b">
+      <c r="AS116" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU116" s="4" t="b">
+      <c r="AU116" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25563,11 +25563,11 @@
       <c r="AK117" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL117" s="4" t="b">
+      <c r="AL117" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM117" s="4" t="b">
+      <c r="AM117" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25583,14 +25583,14 @@
       <c r="AR117" s="2" t="s">
         <v>2290</v>
       </c>
-      <c r="AS117" s="4" t="b">
+      <c r="AS117" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT117" s="2" t="s">
         <v>2291</v>
       </c>
-      <c r="AU117" s="4" t="b">
+      <c r="AU117" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25713,11 +25713,11 @@
       <c r="AK118" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL118" s="4" t="b">
+      <c r="AL118" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM118" s="4" t="b">
+      <c r="AM118" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -25736,14 +25736,14 @@
       <c r="AR118" s="2" t="s">
         <v>2310</v>
       </c>
-      <c r="AS118" s="4" t="b">
+      <c r="AS118" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT118" s="2" t="s">
         <v>2311</v>
       </c>
-      <c r="AU118" s="4" t="b">
+      <c r="AU118" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25860,11 +25860,11 @@
       <c r="AK119" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="AL119" s="4" t="b">
+      <c r="AL119" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM119" s="4" t="b">
+      <c r="AM119" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -25880,14 +25880,14 @@
       <c r="AR119" s="2" t="s">
         <v>2243</v>
       </c>
-      <c r="AS119" s="4" t="b">
+      <c r="AS119" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT119" s="2" t="s">
         <v>2325</v>
       </c>
-      <c r="AU119" s="4" t="b">
+      <c r="AU119" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26007,11 +26007,11 @@
       <c r="AK120" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL120" s="4" t="b">
+      <c r="AL120" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM120" s="4" t="b">
+      <c r="AM120" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26027,11 +26027,11 @@
       <c r="AR120" s="2" t="s">
         <v>1048</v>
       </c>
-      <c r="AS120" s="4" t="b">
+      <c r="AS120" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU120" s="4" t="b">
+      <c r="AU120" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -26157,11 +26157,11 @@
       <c r="AK121" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL121" s="4" t="b">
+      <c r="AL121" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM121" s="4" t="b">
+      <c r="AM121" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26180,11 +26180,11 @@
       <c r="AR121" s="2" t="s">
         <v>1256</v>
       </c>
-      <c r="AS121" s="4" t="b">
+      <c r="AS121" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU121" s="4" t="b">
+      <c r="AU121" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26304,11 +26304,11 @@
       <c r="AK122" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL122" s="4" t="b">
+      <c r="AL122" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM122" s="4" t="b">
+      <c r="AM122" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26324,14 +26324,14 @@
       <c r="AR122" s="2" t="s">
         <v>907</v>
       </c>
-      <c r="AS122" s="4" t="b">
+      <c r="AS122" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT122" s="2" t="s">
         <v>2373</v>
       </c>
-      <c r="AU122" s="4" t="b">
+      <c r="AU122" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26454,11 +26454,11 @@
       <c r="AK123" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL123" s="4" t="b">
+      <c r="AL123" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM123" s="4" t="b">
+      <c r="AM123" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26477,11 +26477,11 @@
       <c r="AR123" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="AS123" s="4" t="b">
+      <c r="AS123" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU123" s="4" t="b">
+      <c r="AU123" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26592,11 +26592,11 @@
       <c r="AK124" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL124" s="4" t="b">
+      <c r="AL124" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM124" s="4" t="b">
+      <c r="AM124" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -26615,11 +26615,11 @@
       <c r="AR124" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="AS124" s="4" t="b">
+      <c r="AS124" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU124" s="4" t="b">
+      <c r="AU124" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26739,11 +26739,11 @@
       <c r="AK125" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL125" s="4" t="b">
+      <c r="AL125" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM125" s="4" t="b">
+      <c r="AM125" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -26759,14 +26759,14 @@
       <c r="AR125" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AS125" s="4" t="b">
+      <c r="AS125" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT125" s="2" t="s">
         <v>2417</v>
       </c>
-      <c r="AU125" s="4" t="b">
+      <c r="AU125" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -26886,11 +26886,11 @@
       <c r="AK126" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL126" s="4" t="b">
+      <c r="AL126" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM126" s="4" t="b">
+      <c r="AM126" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -26909,14 +26909,14 @@
       <c r="AR126" s="2" t="s">
         <v>1524</v>
       </c>
-      <c r="AS126" s="4" t="b">
+      <c r="AS126" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT126" s="2" t="s">
         <v>2434</v>
       </c>
-      <c r="AU126" s="4" t="b">
+      <c r="AU126" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -27030,11 +27030,11 @@
       <c r="AK127" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL127" s="4" t="b">
+      <c r="AL127" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM127" s="4" t="b">
+      <c r="AM127" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -27050,14 +27050,14 @@
       <c r="AR127" s="2" t="s">
         <v>2448</v>
       </c>
-      <c r="AS127" s="4" t="b">
+      <c r="AS127" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT127" s="2" t="s">
         <v>2449</v>
       </c>
-      <c r="AU127" s="4" t="b">
+      <c r="AU127" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -27168,11 +27168,11 @@
       <c r="AK128" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL128" s="4" t="b">
+      <c r="AL128" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM128" s="4" t="b">
+      <c r="AM128" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -27191,11 +27191,11 @@
       <c r="AR128" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AS128" s="4" t="b">
+      <c r="AS128" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU128" s="4" t="b">
+      <c r="AU128" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -27321,11 +27321,11 @@
       <c r="AK129" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL129" s="4" t="b">
+      <c r="AL129" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM129" s="4" t="b">
+      <c r="AM129" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -27341,11 +27341,11 @@
       <c r="AR129" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="AS129" s="4" t="b">
+      <c r="AS129" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU129" s="4" t="b">
+      <c r="AU129" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -27471,11 +27471,11 @@
       <c r="AK130" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="AL130" s="4" t="b">
+      <c r="AL130" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM130" s="4" t="b">
+      <c r="AM130" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -27494,14 +27494,14 @@
       <c r="AR130" s="2" t="s">
         <v>2490</v>
       </c>
-      <c r="AS130" s="4" t="b">
+      <c r="AS130" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT130" s="2" t="s">
         <v>2325</v>
       </c>
-      <c r="AU130" s="4" t="b">
+      <c r="AU130" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -27615,11 +27615,11 @@
       <c r="AK131" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL131" s="4" t="b">
+      <c r="AL131" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM131" s="4" t="b">
+      <c r="AM131" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -27635,11 +27635,11 @@
       <c r="AR131" s="2" t="s">
         <v>2509</v>
       </c>
-      <c r="AS131" s="4" t="b">
+      <c r="AS131" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU131" s="4" t="b">
+      <c r="AU131" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -27759,11 +27759,11 @@
       <c r="AK132" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL132" s="4" t="b">
+      <c r="AL132" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM132" s="4" t="b">
+      <c r="AM132" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -27782,11 +27782,11 @@
       <c r="AR132" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AS132" s="4" t="b">
+      <c r="AS132" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU132" s="4" t="b">
+      <c r="AU132" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -27903,11 +27903,11 @@
       <c r="AK133" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL133" s="4" t="b">
+      <c r="AL133" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM133" s="4" t="b">
+      <c r="AM133" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -27923,11 +27923,11 @@
       <c r="AR133" s="2" t="s">
         <v>2540</v>
       </c>
-      <c r="AS133" s="4" t="b">
+      <c r="AS133" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU133" s="4" t="b">
+      <c r="AU133" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -28053,11 +28053,11 @@
       <c r="AK134" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL134" s="4" t="b">
+      <c r="AL134" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM134" s="4" t="b">
+      <c r="AM134" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -28073,14 +28073,14 @@
       <c r="AR134" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AS134" s="4" t="b">
+      <c r="AS134" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT134" s="2" t="s">
         <v>545</v>
       </c>
-      <c r="AU134" s="4" t="b">
+      <c r="AU134" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -28194,11 +28194,11 @@
       <c r="AK135" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL135" s="4" t="b">
+      <c r="AL135" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM135" s="4" t="b">
+      <c r="AM135" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -28217,14 +28217,14 @@
       <c r="AR135" s="2" t="s">
         <v>1417</v>
       </c>
-      <c r="AS135" s="4" t="b">
+      <c r="AS135" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT135" s="2" t="s">
         <v>2570</v>
       </c>
-      <c r="AU135" s="4" t="b">
+      <c r="AU135" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -28341,11 +28341,11 @@
       <c r="AK136" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL136" s="4" t="b">
+      <c r="AL136" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM136" s="4" t="b">
+      <c r="AM136" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -28364,11 +28364,11 @@
       <c r="AR136" s="2" t="s">
         <v>2584</v>
       </c>
-      <c r="AS136" s="4" t="b">
+      <c r="AS136" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU136" s="4" t="b">
+      <c r="AU136" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -28488,11 +28488,11 @@
       <c r="AK137" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL137" s="4" t="b">
+      <c r="AL137" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AM137" s="4" t="b">
+      <c r="AM137" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -28511,11 +28511,11 @@
       <c r="AR137" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="AS137" s="4" t="b">
+      <c r="AS137" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU137" s="4" t="b">
+      <c r="AU137" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -28632,11 +28632,11 @@
       <c r="AK138" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL138" s="4" t="b">
+      <c r="AL138" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM138" s="4" t="b">
+      <c r="AM138" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -28652,11 +28652,11 @@
       <c r="AR138" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="AS138" s="4" t="b">
+      <c r="AS138" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU138" s="4" t="b">
+      <c r="AU138" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -28779,11 +28779,11 @@
       <c r="AK139" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL139" s="4" t="b">
+      <c r="AL139" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM139" s="4" t="b">
+      <c r="AM139" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -28799,14 +28799,14 @@
       <c r="AR139" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="AS139" s="4" t="b">
+      <c r="AS139" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="AT139" s="2" t="s">
         <v>2634</v>
       </c>
-      <c r="AU139" s="4" t="b">
+      <c r="AU139" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -28935,11 +28935,11 @@
       <c r="AK140" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL140" s="4" t="b">
+      <c r="AL140" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM140" s="4" t="b">
+      <c r="AM140" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -28955,11 +28955,11 @@
       <c r="AR140" s="2" t="s">
         <v>1256</v>
       </c>
-      <c r="AS140" s="4" t="b">
+      <c r="AS140" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU140" s="4" t="b">
+      <c r="AU140" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -29064,11 +29064,11 @@
       <c r="AK141" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="AL141" s="4" t="b">
+      <c r="AL141" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM141" s="4" t="b">
+      <c r="AM141" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -29084,11 +29084,11 @@
       <c r="AR141" s="2" t="s">
         <v>2667</v>
       </c>
-      <c r="AS141" s="4" t="b">
+      <c r="AS141" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU141" s="4" t="b">
+      <c r="AU141" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -29211,11 +29211,11 @@
       <c r="AK142" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AL142" s="4" t="b">
+      <c r="AL142" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="AM142" s="4" t="b">
+      <c r="AM142" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -29231,11 +29231,11 @@
       <c r="AR142" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="AS142" s="4" t="b">
+      <c r="AS142" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AU142" s="4" t="b">
+      <c r="AU142" s="1" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Add the articles title again
</commit_message>
<xml_diff>
--- a/datasets/Cleaned_data.xlsx
+++ b/datasets/Cleaned_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\openSUSE-Tumbleweed\home\leo\VCodeProjects\Analisis\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DA7CEA-DCA9-4A6E-88B3-2162FB760F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC492B7-76DD-4F08-ACC5-C52A1956A5E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8861,11 +8861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:BC143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AR21" sqref="AR21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9085,7 +9084,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -9235,7 +9234,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>86</v>
       </c>
@@ -9397,7 +9396,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>119</v>
       </c>
@@ -9556,7 +9555,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>530</v>
       </c>
@@ -9715,7 +9714,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="6" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>174</v>
       </c>
@@ -9871,7 +9870,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>199</v>
       </c>
@@ -10030,7 +10029,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>220</v>
       </c>
@@ -10192,7 +10191,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="9" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>249</v>
       </c>
@@ -10348,7 +10347,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="10" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>278</v>
       </c>
@@ -10660,7 +10659,7 @@
         <v>1590</v>
       </c>
     </row>
-    <row r="12" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>324</v>
       </c>
@@ -10813,7 +10812,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="13" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>343</v>
       </c>
@@ -10966,7 +10965,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="14" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>369</v>
       </c>
@@ -11119,7 +11118,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="15" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>393</v>
       </c>
@@ -11269,7 +11268,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="16" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>409</v>
       </c>
@@ -11431,7 +11430,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="17" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>433</v>
       </c>
@@ -11587,7 +11586,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="18" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>455</v>
       </c>
@@ -11749,7 +11748,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="19" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>482</v>
       </c>
@@ -11911,7 +11910,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="20" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>504</v>
       </c>
@@ -12220,7 +12219,7 @@
         <v>2705</v>
       </c>
     </row>
-    <row r="22" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>550</v>
       </c>
@@ -12376,7 +12375,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="23" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>569</v>
       </c>
@@ -12532,7 +12531,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="24" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>592</v>
       </c>
@@ -12688,7 +12687,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="25" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>612</v>
       </c>
@@ -12844,7 +12843,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="26" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>634</v>
       </c>
@@ -13003,7 +13002,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="27" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>665</v>
       </c>
@@ -13162,7 +13161,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="28" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>689</v>
       </c>
@@ -13327,7 +13326,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="29" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>2146</v>
       </c>
@@ -13477,7 +13476,7 @@
         <v>2162</v>
       </c>
     </row>
-    <row r="30" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>740</v>
       </c>
@@ -13633,7 +13632,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="31" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>759</v>
       </c>
@@ -13789,7 +13788,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="32" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>778</v>
       </c>
@@ -13942,7 +13941,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="33" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>2239</v>
       </c>
@@ -14095,7 +14094,7 @@
         <v>2260</v>
       </c>
     </row>
-    <row r="34" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>810</v>
       </c>
@@ -14251,7 +14250,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="35" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>2278</v>
       </c>
@@ -14404,7 +14403,7 @@
         <v>2291</v>
       </c>
     </row>
-    <row r="36" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>851</v>
       </c>
@@ -14560,7 +14559,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="37" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>867</v>
       </c>
@@ -14722,7 +14721,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="38" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>885</v>
       </c>
@@ -14884,7 +14883,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="39" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>906</v>
       </c>
@@ -15049,7 +15048,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="40" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -15211,7 +15210,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="41" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>944</v>
       </c>
@@ -15364,7 +15363,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="42" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>959</v>
       </c>
@@ -15526,7 +15525,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="43" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>1262</v>
       </c>
@@ -15676,7 +15675,7 @@
         <v>1284</v>
       </c>
     </row>
-    <row r="44" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>998</v>
       </c>
@@ -15835,7 +15834,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="45" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>1018</v>
       </c>
@@ -15988,7 +15987,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="46" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>2308</v>
       </c>
@@ -16147,7 +16146,7 @@
         <v>2328</v>
       </c>
     </row>
-    <row r="47" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>1059</v>
       </c>
@@ -16300,7 +16299,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="48" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>1075</v>
       </c>
@@ -16456,7 +16455,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="49" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>1092</v>
       </c>
@@ -16615,7 +16614,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="50" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>1110</v>
       </c>
@@ -16765,7 +16764,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="51" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>550</v>
       </c>
@@ -16924,7 +16923,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="52" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>1142</v>
       </c>
@@ -17071,7 +17070,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="53" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>1158</v>
       </c>
@@ -17233,7 +17232,7 @@
         <v>1181</v>
       </c>
     </row>
-    <row r="54" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>1182</v>
       </c>
@@ -17398,7 +17397,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="55" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>1200</v>
       </c>
@@ -17557,7 +17556,7 @@
         <v>1217</v>
       </c>
     </row>
-    <row r="56" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>1218</v>
       </c>
@@ -17710,7 +17709,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="57" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>1235</v>
       </c>
@@ -17866,7 +17865,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="58" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>2760</v>
       </c>
@@ -18016,7 +18015,7 @@
         <v>2773</v>
       </c>
     </row>
-    <row r="59" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>1285</v>
       </c>
@@ -18166,7 +18165,7 @@
         <v>1308</v>
       </c>
     </row>
-    <row r="60" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>1309</v>
       </c>
@@ -18319,7 +18318,7 @@
         <v>1325</v>
       </c>
     </row>
-    <row r="61" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>1326</v>
       </c>
@@ -18478,7 +18477,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="62" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>828</v>
       </c>
@@ -18634,7 +18633,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="63" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>1372</v>
       </c>
@@ -18940,7 +18939,7 @@
         <v>1403</v>
       </c>
     </row>
-    <row r="65" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>1404</v>
       </c>
@@ -19090,7 +19089,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="66" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>1421</v>
       </c>
@@ -19243,7 +19242,7 @@
         <v>1437</v>
       </c>
     </row>
-    <row r="67" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>1438</v>
       </c>
@@ -19390,7 +19389,7 @@
         <v>1459</v>
       </c>
     </row>
-    <row r="68" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>1460</v>
       </c>
@@ -19546,7 +19545,7 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="69" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>1477</v>
       </c>
@@ -19702,7 +19701,7 @@
         <v>1494</v>
       </c>
     </row>
-    <row r="70" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>1495</v>
       </c>
@@ -19864,7 +19863,7 @@
         <v>1517</v>
       </c>
     </row>
-    <row r="71" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>1518</v>
       </c>
@@ -20026,7 +20025,7 @@
         <v>1536</v>
       </c>
     </row>
-    <row r="72" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>1537</v>
       </c>
@@ -20176,7 +20175,7 @@
         <v>1555</v>
       </c>
     </row>
-    <row r="73" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>1556</v>
       </c>
@@ -20335,7 +20334,7 @@
         <v>1573</v>
       </c>
     </row>
-    <row r="74" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>1775</v>
       </c>
@@ -20656,7 +20655,7 @@
         <v>1614</v>
       </c>
     </row>
-    <row r="76" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>1615</v>
       </c>
@@ -20815,7 +20814,7 @@
         <v>1637</v>
       </c>
     </row>
-    <row r="77" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>1638</v>
       </c>
@@ -20974,7 +20973,7 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="78" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>1661</v>
       </c>
@@ -21133,7 +21132,7 @@
         <v>1678</v>
       </c>
     </row>
-    <row r="79" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>1679</v>
       </c>
@@ -21289,7 +21288,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="80" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>1701</v>
       </c>
@@ -21439,7 +21438,7 @@
         <v>1715</v>
       </c>
     </row>
-    <row r="81" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>1716</v>
       </c>
@@ -21604,7 +21603,7 @@
         <v>1735</v>
       </c>
     </row>
-    <row r="82" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>1736</v>
       </c>
@@ -21760,7 +21759,7 @@
         <v>1759</v>
       </c>
     </row>
-    <row r="83" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>1760</v>
       </c>
@@ -21913,7 +21912,7 @@
         <v>1774</v>
       </c>
     </row>
-    <row r="84" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>2626</v>
       </c>
@@ -22063,7 +22062,7 @@
         <v>2640</v>
       </c>
     </row>
-    <row r="85" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>1793</v>
       </c>
@@ -22222,7 +22221,7 @@
         <v>1808</v>
       </c>
     </row>
-    <row r="86" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>1809</v>
       </c>
@@ -22381,7 +22380,7 @@
         <v>1824</v>
       </c>
     </row>
-    <row r="87" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>1825</v>
       </c>
@@ -22531,7 +22530,7 @@
         <v>1846</v>
       </c>
     </row>
-    <row r="88" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>1847</v>
       </c>
@@ -22669,7 +22668,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>1866</v>
       </c>
@@ -22831,7 +22830,7 @@
         <v>1881</v>
       </c>
     </row>
-    <row r="90" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>1882</v>
       </c>
@@ -22987,7 +22986,7 @@
         <v>1898</v>
       </c>
     </row>
-    <row r="91" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>1899</v>
       </c>
@@ -23146,7 +23145,7 @@
         <v>1919</v>
       </c>
     </row>
-    <row r="92" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>1920</v>
       </c>
@@ -23305,7 +23304,7 @@
         <v>1937</v>
       </c>
     </row>
-    <row r="93" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>1938</v>
       </c>
@@ -23464,7 +23463,7 @@
         <v>1963</v>
       </c>
     </row>
-    <row r="94" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>1964</v>
       </c>
@@ -23629,7 +23628,7 @@
         <v>1984</v>
       </c>
     </row>
-    <row r="95" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>1985</v>
       </c>
@@ -23788,7 +23787,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="96" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>2004</v>
       </c>
@@ -23938,7 +23937,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="97" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>2016</v>
       </c>
@@ -24097,7 +24096,7 @@
         <v>2034</v>
       </c>
     </row>
-    <row r="98" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>2035</v>
       </c>
@@ -24259,7 +24258,7 @@
         <v>2058</v>
       </c>
     </row>
-    <row r="99" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>2059</v>
       </c>
@@ -24412,7 +24411,7 @@
         <v>2079</v>
       </c>
     </row>
-    <row r="100" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>2080</v>
       </c>
@@ -24565,7 +24564,7 @@
         <v>2090</v>
       </c>
     </row>
-    <row r="101" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>2091</v>
       </c>
@@ -24715,7 +24714,7 @@
         <v>2106</v>
       </c>
     </row>
-    <row r="102" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>2107</v>
       </c>
@@ -24865,7 +24864,7 @@
         <v>2130</v>
       </c>
     </row>
-    <row r="103" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>2131</v>
       </c>
@@ -25021,7 +25020,7 @@
         <v>2145</v>
       </c>
     </row>
-    <row r="104" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>2774</v>
       </c>
@@ -25162,7 +25161,7 @@
         <v>2793</v>
       </c>
     </row>
-    <row r="105" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>2163</v>
       </c>
@@ -25309,7 +25308,7 @@
         <v>2177</v>
       </c>
     </row>
-    <row r="106" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>2178</v>
       </c>
@@ -25474,7 +25473,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="107" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>2201</v>
       </c>
@@ -25627,7 +25626,7 @@
         <v>2216</v>
       </c>
     </row>
-    <row r="108" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>2217</v>
       </c>
@@ -25789,7 +25788,7 @@
         <v>2238</v>
       </c>
     </row>
-    <row r="109" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>927</v>
       </c>
@@ -25936,7 +25935,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="110" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>2261</v>
       </c>
@@ -26098,7 +26097,7 @@
         <v>2277</v>
       </c>
     </row>
-    <row r="111" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>1351</v>
       </c>
@@ -26257,7 +26256,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="112" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>2292</v>
       </c>
@@ -26416,7 +26415,7 @@
         <v>2307</v>
       </c>
     </row>
-    <row r="113" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>302</v>
       </c>
@@ -26578,7 +26577,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="114" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>2329</v>
       </c>
@@ -26725,7 +26724,7 @@
         <v>2343</v>
       </c>
     </row>
-    <row r="115" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>2344</v>
       </c>
@@ -26872,7 +26871,7 @@
         <v>2365</v>
       </c>
     </row>
-    <row r="116" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>2366</v>
       </c>
@@ -27022,7 +27021,7 @@
         <v>2379</v>
       </c>
     </row>
-    <row r="117" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>2380</v>
       </c>
@@ -27175,7 +27174,7 @@
         <v>2394</v>
       </c>
     </row>
-    <row r="118" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>2395</v>
       </c>
@@ -27334,7 +27333,7 @@
         <v>2416</v>
       </c>
     </row>
-    <row r="119" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>2417</v>
       </c>
@@ -27484,7 +27483,7 @@
         <v>2429</v>
       </c>
     </row>
-    <row r="120" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>2430</v>
       </c>
@@ -27637,7 +27636,7 @@
         <v>2447</v>
       </c>
     </row>
-    <row r="121" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>2448</v>
       </c>
@@ -27793,7 +27792,7 @@
         <v>2463</v>
       </c>
     </row>
-    <row r="122" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>2464</v>
       </c>
@@ -27946,7 +27945,7 @@
         <v>2480</v>
       </c>
     </row>
-    <row r="123" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>2481</v>
       </c>
@@ -28108,7 +28107,7 @@
         <v>2498</v>
       </c>
     </row>
-    <row r="124" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>2499</v>
       </c>
@@ -28255,7 +28254,7 @@
         <v>2512</v>
       </c>
     </row>
-    <row r="125" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>2513</v>
       </c>
@@ -28411,7 +28410,7 @@
         <v>2527</v>
       </c>
     </row>
-    <row r="126" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>2528</v>
       </c>
@@ -28567,7 +28566,7 @@
         <v>2545</v>
       </c>
     </row>
-    <row r="127" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>2546</v>
       </c>
@@ -28714,7 +28713,7 @@
         <v>2561</v>
       </c>
     </row>
-    <row r="128" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>2562</v>
       </c>
@@ -28861,7 +28860,7 @@
         <v>2575</v>
       </c>
     </row>
-    <row r="129" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>2576</v>
       </c>
@@ -29017,7 +29016,7 @@
         <v>2591</v>
       </c>
     </row>
-    <row r="130" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>2592</v>
       </c>
@@ -29182,7 +29181,7 @@
         <v>2604</v>
       </c>
     </row>
-    <row r="131" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>2605</v>
       </c>
@@ -29326,7 +29325,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="132" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>795</v>
       </c>
@@ -29488,7 +29487,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="133" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>2641</v>
       </c>
@@ -29641,7 +29640,7 @@
         <v>2658</v>
       </c>
     </row>
-    <row r="134" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>2659</v>
       </c>
@@ -29797,7 +29796,7 @@
         <v>2671</v>
       </c>
     </row>
-    <row r="135" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>2672</v>
       </c>
@@ -29947,7 +29946,7 @@
         <v>2689</v>
       </c>
     </row>
-    <row r="136" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>1035</v>
       </c>
@@ -30106,7 +30105,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="137" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>2706</v>
       </c>
@@ -30262,7 +30261,7 @@
         <v>2721</v>
       </c>
     </row>
-    <row r="138" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>2722</v>
       </c>
@@ -30409,7 +30408,7 @@
         <v>2740</v>
       </c>
     </row>
-    <row r="139" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>2741</v>
       </c>
@@ -30571,7 +30570,7 @@
         <v>2759</v>
       </c>
     </row>
-    <row r="140" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>713</v>
       </c>
@@ -30721,7 +30720,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="141" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>979</v>
       </c>
@@ -30880,7 +30879,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="142" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>2794</v>
       </c>
@@ -31033,7 +31032,7 @@
         <v>2809</v>
       </c>
     </row>
-    <row r="143" spans="1:55" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>2810</v>
       </c>
@@ -31190,14 +31189,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BC143" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="43">
-      <filters>
-        <filter val="Activity estimation"/>
-        <filter val="Passengers flow"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>